<commit_message>
Pawn quick info 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Pawn quick info - 3078081326/Pawn quick info - 3078081326.xlsx
+++ b/Data/Pawn quick info - 3078081326/Pawn quick info - 3078081326.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\Pawn quick info - 3078081326\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D9AA64-A9A3-4E49-89B4-0619D2E92547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10A878-730B-4DE7-9922-DFF064F9D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,12 +311,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="E36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-05-21에 새로 추가된 노드들 (1개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="141">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -345,6 +358,9 @@
     <t>PawnQuickInfoSettingsCategory</t>
   </si>
   <si>
+    <t>Pawn Quick Info</t>
+  </si>
+  <si>
     <t>- Pawn Quick Info -</t>
   </si>
   <si>
@@ -354,6 +370,9 @@
     <t>ShowCustomHediffMenu</t>
   </si>
   <si>
+    <t>Show custom damage menu</t>
+  </si>
+  <si>
     <t>커스텀 피해 메뉴 표시</t>
   </si>
   <si>
@@ -363,6 +382,9 @@
     <t>EnableCameraJump</t>
   </si>
   <si>
+    <t>Enable camera jump</t>
+  </si>
+  <si>
     <t>카메라 이동 활성화</t>
   </si>
   <si>
@@ -372,6 +394,9 @@
     <t>EnableCameraJumpTooltip</t>
   </si>
   <si>
+    <t>If enabled, special menu actions [Shift + LMB] will move camera to requested pawn</t>
+  </si>
+  <si>
     <t>활성화된 경우, 특수 메뉴 동작 [Shift + LMB]를 통해 카메라를 요청된 폰으로 이동합니다.</t>
   </si>
   <si>
@@ -381,6 +406,9 @@
     <t>ShowTraderInfo</t>
   </si>
   <si>
+    <t>Show trader menu</t>
+  </si>
+  <si>
     <t>트레이더 메뉴 표시</t>
   </si>
   <si>
@@ -390,6 +418,9 @@
     <t>EnableShiftButton</t>
   </si>
   <si>
+    <t>Enable sticking with [Shift] key</t>
+  </si>
+  <si>
     <t>[Shift] 키로 고정 활성화</t>
   </si>
   <si>
@@ -399,6 +430,9 @@
     <t>OnlyIfPawnSelected</t>
   </si>
   <si>
+    <t>Menu shows only when pawn selected</t>
+  </si>
+  <si>
     <t>폰을 선택한 경우에만 메뉴가 표시됩니다.</t>
   </si>
   <si>
@@ -408,6 +442,9 @@
     <t>ForAll</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>전체</t>
   </si>
   <si>
@@ -417,6 +454,9 @@
     <t>ForPlayerAndHostile</t>
   </si>
   <si>
+    <t>Player and hostiles</t>
+  </si>
+  <si>
     <t>플레이어 및 적</t>
   </si>
   <si>
@@ -426,6 +466,9 @@
     <t>ForPlayerAndAllies</t>
   </si>
   <si>
+    <t>Player and allies</t>
+  </si>
+  <si>
     <t>플레이어 및 아군</t>
   </si>
   <si>
@@ -435,6 +478,9 @@
     <t>OnlyForPlayer</t>
   </si>
   <si>
+    <t>Only player</t>
+  </si>
+  <si>
     <t>플레이어만</t>
   </si>
   <si>
@@ -444,18 +490,51 @@
     <t>HediffModeInfo</t>
   </si>
   <si>
+    <t>Pawn status menu is enabled for:</t>
+  </si>
+  <si>
     <t>Keyed+CommonModeInfo</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>폰 상태 메뉴를 활성화 합니다:</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>CommonModeInfo</t>
   </si>
   <si>
+    <t>Pawn skills menu is enabled for:</t>
+  </si>
+  <si>
     <t>Keyed+ActivationModeInfo</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>폰 기술 메뉴를 활성화 합니다:</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ActivationModeInfo</t>
   </si>
   <si>
+    <t>Menu activation mode:</t>
+  </si>
+  <si>
     <t>메뉴 활성화 모드:</t>
   </si>
   <si>
@@ -474,6 +553,9 @@
     <t>DelayedTooltip</t>
   </si>
   <si>
+    <t>Kind of like how tooltips work. There is a slight delay before they appear</t>
+  </si>
+  <si>
     <t>툴팁이 작동하는 방식과 비슷합니다. 표시되기까지 약간의 지연이 있습니다.</t>
   </si>
   <si>
@@ -492,6 +574,9 @@
     <t>InstantTooltip</t>
   </si>
   <si>
+    <t>Appears instantly when hovering over a pawn</t>
+  </si>
+  <si>
     <t>폰 위로 마우스를 가져가면 즉시 표시됩니다.</t>
   </si>
   <si>
@@ -501,6 +586,9 @@
     <t>EnableDollZoom</t>
   </si>
   <si>
+    <t>Enable hediff doll zoom</t>
+  </si>
+  <si>
     <t>헤디프 인형 확대/축소 사용</t>
   </si>
   <si>
@@ -510,6 +598,9 @@
     <t>EnableDollZoomTooltip</t>
   </si>
   <si>
+    <t>If enabled, you can zoom hediff doll when hover mouse while hold [Shift]</t>
+  </si>
+  <si>
     <t>활성화하면 [Shift] 키를 누른 상태에서 마우스를 가리키면 헤디프 인형을 확대/축소할 수 있습니다.</t>
   </si>
   <si>
@@ -519,66 +610,12 @@
     <t>EnableColonistBar</t>
   </si>
   <si>
+    <t>Enable menu on colonist bar</t>
+  </si>
+  <si>
     <t>정착민 바에 메뉴 활성화</t>
   </si>
   <si>
-    <t>Pawn Quick Info</t>
-  </si>
-  <si>
-    <t>Show custom damage menu</t>
-  </si>
-  <si>
-    <t>Enable camera jump</t>
-  </si>
-  <si>
-    <t>If enabled, special menu actions [Shift + LMB] will move camera to requested pawn</t>
-  </si>
-  <si>
-    <t>Show trader menu</t>
-  </si>
-  <si>
-    <t>Enable sticking with [Shift] key</t>
-  </si>
-  <si>
-    <t>Menu shows only when pawn selected</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Player and hostiles</t>
-  </si>
-  <si>
-    <t>Player and allies</t>
-  </si>
-  <si>
-    <t>Only player</t>
-  </si>
-  <si>
-    <t>Pawn status menu is enabled for:</t>
-  </si>
-  <si>
-    <t>Pawn skills menu is enabled for:</t>
-  </si>
-  <si>
-    <t>Menu activation mode:</t>
-  </si>
-  <si>
-    <t>Kind of like how tooltips work. There is a slight delay before they appear</t>
-  </si>
-  <si>
-    <t>Appears instantly when hovering over a pawn</t>
-  </si>
-  <si>
-    <t>Enable hediff doll zoom</t>
-  </si>
-  <si>
-    <t>If enabled, you can zoom hediff doll when hover mouse while hold [Shift]</t>
-  </si>
-  <si>
-    <t>Enable menu on colonist bar</t>
-  </si>
-  <si>
     <t>Keyed+CurrentJobModeInfo</t>
   </si>
   <si>
@@ -591,12 +628,27 @@
     <t>Keyed+EnableTinyFont</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>현재 작업을 표시합니다:</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>EnableTinyFont</t>
   </si>
   <si>
     <t>Enable tiny font</t>
   </si>
   <si>
+    <t>작은 글꼴 활성화</t>
+  </si>
+  <si>
     <t>Keyed+EnableItemInfo</t>
   </si>
   <si>
@@ -606,6 +658,9 @@
     <t>Enable item tooltips</t>
   </si>
   <si>
+    <t>아이템 툴팁 활성화</t>
+  </si>
+  <si>
     <t>Keyed+EnableBuildingInfo</t>
   </si>
   <si>
@@ -618,12 +673,27 @@
     <t>Keyed+Delayedx2</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>건물 툴팁 활성화</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Delayedx2</t>
   </si>
   <si>
     <t>Delayed (1 sec)</t>
   </si>
   <si>
+    <t>지연(1초)</t>
+  </si>
+  <si>
     <t>Keyed+DelayedTooltipx2</t>
   </si>
   <si>
@@ -636,12 +706,27 @@
     <t>Keyed+HoldButton</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>깜박거리는게 마음에 들지 않는 경우</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>HoldButton</t>
   </si>
   <si>
     <t>Hold button\n(Shift)</t>
   </si>
   <si>
+    <t>길게 누르기\n(Shift)</t>
+  </si>
+  <si>
     <t>Keyed+ForAllExceptPlayer</t>
   </si>
   <si>
@@ -651,6 +736,9 @@
     <t>All except player</t>
   </si>
   <si>
+    <t>플레이어 제외</t>
+  </si>
+  <si>
     <t>Keyed+ForHostile</t>
   </si>
   <si>
@@ -663,6 +751,18 @@
     <t>Keyed+ForAllies</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>적</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ForAllies</t>
   </si>
   <si>
@@ -672,12 +772,27 @@
     <t>Keyed+CurrentWeaponModeInfo</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>동맹</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>CurrentWeaponModeInfo</t>
   </si>
   <si>
     <t>Equipped weapon is shown for:</t>
   </si>
   <si>
+    <t>장착한 무기를 표시합니다:</t>
+  </si>
+  <si>
     <t>Keyed+EnableHoldingWeaponInfo</t>
   </si>
   <si>
@@ -687,53 +802,19 @@
     <t>Enable equipped weapon info</t>
   </si>
   <si>
-    <t>작은 글꼴 활성화</t>
-  </si>
-  <si>
-    <t>아이템 툴팁 활성화</t>
-  </si>
-  <si>
-    <t>지연(1초)</t>
-  </si>
-  <si>
-    <t>깜박거리는게 마음에 들지 않는 경우</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>길게 누르기\n(Shift)</t>
-  </si>
-  <si>
-    <t>플레이어 제외</t>
-  </si>
-  <si>
-    <t>적</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>동맹</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>장착한 무기를 표시합니다:</t>
-  </si>
-  <si>
     <t>장착 무기 정보 활성화</t>
   </si>
   <si>
-    <t>현재 작업을 표시합니다:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>폰 상태 메뉴를 활성화 합니다:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>폰 기술 메뉴를 활성화 합니다:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>건물 툴팁 활성화</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>Keyed+ShowOrganProsthesis</t>
+  </si>
+  <si>
+    <t>ShowOrganProsthesis</t>
+  </si>
+  <si>
+    <t>Show organs prosthesis</t>
+  </si>
+  <si>
+    <t>장기 보철물 표시</t>
   </si>
 </sst>
 </file>
@@ -1103,16 +1184,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="40.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1146,554 +1229,571 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>